<commit_message>
TODO no. 5 done
</commit_message>
<xml_diff>
--- a/Capacity_Comparison_Flat.xlsx
+++ b/Capacity_Comparison_Flat.xlsx
@@ -29,12 +29,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFA500"/>
+        <bgColor rgb="00FFA500"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -495,7 +502,6 @@
       <c r="F2" t="n">
         <v>-12</v>
       </c>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -522,7 +528,6 @@
       <c r="F3" t="n">
         <v>-1</v>
       </c>
-      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -549,7 +554,6 @@
       <c r="F4" t="n">
         <v>-7</v>
       </c>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,7 +580,6 @@
       <c r="F5" t="n">
         <v>-32</v>
       </c>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -603,31 +606,30 @@
       <c r="F6" t="n">
         <v>32</v>
       </c>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>2144</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
@@ -659,7 +661,6 @@
       <c r="F8" t="n">
         <v>-16</v>
       </c>
-      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -686,7 +687,6 @@
       <c r="F9" t="n">
         <v>17</v>
       </c>
-      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -713,7 +713,6 @@
       <c r="F10" t="n">
         <v>30.3</v>
       </c>
-      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -740,7 +739,6 @@
       <c r="F11" t="n">
         <v>-11</v>
       </c>
-      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -767,31 +765,30 @@
       <c r="F12" t="n">
         <v>24.5</v>
       </c>
-      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>2144</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
@@ -823,7 +820,6 @@
       <c r="F14" t="n">
         <v>0</v>
       </c>
-      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -850,7 +846,6 @@
       <c r="F15" t="n">
         <v>-32</v>
       </c>
-      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -877,7 +872,6 @@
       <c r="F16" t="n">
         <v>0.5</v>
       </c>
-      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -904,31 +898,30 @@
       <c r="F17" t="n">
         <v>31.5</v>
       </c>
-      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>2144</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
@@ -960,7 +953,6 @@
       <c r="F19" t="n">
         <v>-16</v>
       </c>
-      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -987,7 +979,6 @@
       <c r="F20" t="n">
         <v>-6</v>
       </c>
-      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1014,7 +1005,6 @@
       <c r="F21" t="n">
         <v>33.5</v>
       </c>
-      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1041,7 +1031,6 @@
       <c r="F22" t="n">
         <v>-96</v>
       </c>
-      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1097,7 +1086,6 @@
       <c r="F24" t="n">
         <v>-39</v>
       </c>
-      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1124,31 +1112,30 @@
       <c r="F25" t="n">
         <v>95</v>
       </c>
-      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>2441</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="n">
+      <c r="D26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="n">
@@ -1180,31 +1167,30 @@
       <c r="F27" t="n">
         <v>152</v>
       </c>
-      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>2441</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="n">
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="n">
@@ -1236,31 +1222,30 @@
       <c r="F29" t="n">
         <v>152</v>
       </c>
-      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
         <is>
           <t>2441</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E30" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
@@ -1292,7 +1277,6 @@
       <c r="F31" t="n">
         <v>2</v>
       </c>
-      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1319,7 +1303,6 @@
       <c r="F32" t="n">
         <v>2</v>
       </c>
-      <c r="G32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1346,7 +1329,6 @@
       <c r="F33" t="n">
         <v>-16</v>
       </c>
-      <c r="G33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1373,7 +1355,6 @@
       <c r="F34" t="n">
         <v>3.5</v>
       </c>
-      <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1400,7 +1381,6 @@
       <c r="F35" t="n">
         <v>1</v>
       </c>
-      <c r="G35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1427,31 +1407,30 @@
       <c r="F36" t="n">
         <v>138</v>
       </c>
-      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>2441</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
+      <c r="E37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G37" t="n">
@@ -1483,7 +1462,6 @@
       <c r="F38" t="n">
         <v>0.5</v>
       </c>
-      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1510,7 +1488,6 @@
       <c r="F39" t="n">
         <v>0.5</v>
       </c>
-      <c r="G39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1537,7 +1514,6 @@
       <c r="F40" t="n">
         <v>0.5</v>
       </c>
-      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1564,7 +1540,6 @@
       <c r="F41" t="n">
         <v>0.5</v>
       </c>
-      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1591,7 +1566,6 @@
       <c r="F42" t="n">
         <v>4</v>
       </c>
-      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1618,7 +1592,6 @@
       <c r="F43" t="n">
         <v>1</v>
       </c>
-      <c r="G43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1645,7 +1618,6 @@
       <c r="F44" t="n">
         <v>0.5</v>
       </c>
-      <c r="G44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1672,7 +1644,6 @@
       <c r="F45" t="n">
         <v>2</v>
       </c>
-      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1699,7 +1670,6 @@
       <c r="F46" t="n">
         <v>1</v>
       </c>
-      <c r="G46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1726,7 +1696,6 @@
       <c r="F47" t="n">
         <v>0.5</v>
       </c>
-      <c r="G47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1753,7 +1722,6 @@
       <c r="F48" t="n">
         <v>0.5</v>
       </c>
-      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1780,7 +1748,6 @@
       <c r="F49" t="n">
         <v>-1</v>
       </c>
-      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1807,7 +1774,6 @@
       <c r="F50" t="n">
         <v>0.5</v>
       </c>
-      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1834,7 +1800,6 @@
       <c r="F51" t="n">
         <v>1.5</v>
       </c>
-      <c r="G51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1861,7 +1826,6 @@
       <c r="F52" t="n">
         <v>0.5</v>
       </c>
-      <c r="G52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1888,7 +1852,6 @@
       <c r="F53" t="n">
         <v>3</v>
       </c>
-      <c r="G53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1915,7 +1878,6 @@
       <c r="F54" t="n">
         <v>4</v>
       </c>
-      <c r="G54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1942,7 +1904,6 @@
       <c r="F55" t="n">
         <v>0.5</v>
       </c>
-      <c r="G55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1969,7 +1930,6 @@
       <c r="F56" t="n">
         <v>0.5</v>
       </c>
-      <c r="G56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1996,7 +1956,6 @@
       <c r="F57" t="n">
         <v>0.5</v>
       </c>
-      <c r="G57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2023,7 +1982,6 @@
       <c r="F58" t="n">
         <v>-94</v>
       </c>
-      <c r="G58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2050,7 +2008,6 @@
       <c r="F59" t="n">
         <v>-16.5</v>
       </c>
-      <c r="G59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2077,31 +2034,30 @@
       <c r="F60" t="n">
         <v>48</v>
       </c>
-      <c r="G60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>2456</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>2456</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="C61" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" t="n">
+      <c r="D61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F61" t="n">
+      <c r="F61" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G61" t="n">
@@ -2133,7 +2089,6 @@
       <c r="F62" t="n">
         <v>0.5</v>
       </c>
-      <c r="G62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2160,7 +2115,6 @@
       <c r="F63" t="n">
         <v>3</v>
       </c>
-      <c r="G63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2187,7 +2141,6 @@
       <c r="F64" t="n">
         <v>6</v>
       </c>
-      <c r="G64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2214,7 +2167,6 @@
       <c r="F65" t="n">
         <v>0.5</v>
       </c>
-      <c r="G65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2241,7 +2193,6 @@
       <c r="F66" t="n">
         <v>0.5</v>
       </c>
-      <c r="G66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2268,7 +2219,6 @@
       <c r="F67" t="n">
         <v>0.5</v>
       </c>
-      <c r="G67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2295,7 +2245,6 @@
       <c r="F68" t="n">
         <v>0.5</v>
       </c>
-      <c r="G68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2322,7 +2271,6 @@
       <c r="F69" t="n">
         <v>0.5</v>
       </c>
-      <c r="G69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2349,7 +2297,6 @@
       <c r="F70" t="n">
         <v>2</v>
       </c>
-      <c r="G70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2376,7 +2323,6 @@
       <c r="F71" t="n">
         <v>0.5</v>
       </c>
-      <c r="G71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2403,7 +2349,6 @@
       <c r="F72" t="n">
         <v>0.5</v>
       </c>
-      <c r="G72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2430,7 +2375,6 @@
       <c r="F73" t="n">
         <v>2.5</v>
       </c>
-      <c r="G73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2457,7 +2401,6 @@
       <c r="F74" t="n">
         <v>7.5</v>
       </c>
-      <c r="G74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2484,7 +2427,6 @@
       <c r="F75" t="n">
         <v>0.5</v>
       </c>
-      <c r="G75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2511,7 +2453,6 @@
       <c r="F76" t="n">
         <v>0.5</v>
       </c>
-      <c r="G76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2538,7 +2479,6 @@
       <c r="F77" t="n">
         <v>-28</v>
       </c>
-      <c r="G77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2565,7 +2505,6 @@
       <c r="F78" t="n">
         <v>4</v>
       </c>
-      <c r="G78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2592,31 +2531,30 @@
       <c r="F79" t="n">
         <v>62</v>
       </c>
-      <c r="G79" t="inlineStr"/>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>2456</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>2456</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="C80" s="2" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="D80" t="n">
-        <v>0</v>
-      </c>
-      <c r="E80" t="n">
+      <c r="D80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F80" t="n">
+      <c r="F80" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G80" t="n">
@@ -2648,7 +2586,6 @@
       <c r="F81" t="n">
         <v>0.5</v>
       </c>
-      <c r="G81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2675,7 +2612,6 @@
       <c r="F82" t="n">
         <v>0.5</v>
       </c>
-      <c r="G82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2702,7 +2638,6 @@
       <c r="F83" t="n">
         <v>0.5</v>
       </c>
-      <c r="G83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2729,7 +2664,6 @@
       <c r="F84" t="n">
         <v>0.5</v>
       </c>
-      <c r="G84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2756,7 +2690,6 @@
       <c r="F85" t="n">
         <v>0.5</v>
       </c>
-      <c r="G85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2783,7 +2716,6 @@
       <c r="F86" t="n">
         <v>0.5</v>
       </c>
-      <c r="G86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2810,7 +2742,6 @@
       <c r="F87" t="n">
         <v>0.5</v>
       </c>
-      <c r="G87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2837,7 +2768,6 @@
       <c r="F88" t="n">
         <v>0.5</v>
       </c>
-      <c r="G88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2864,7 +2794,6 @@
       <c r="F89" t="n">
         <v>1</v>
       </c>
-      <c r="G89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2891,7 +2820,6 @@
       <c r="F90" t="n">
         <v>0.5</v>
       </c>
-      <c r="G90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2918,7 +2846,6 @@
       <c r="F91" t="n">
         <v>0.5</v>
       </c>
-      <c r="G91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2945,7 +2872,6 @@
       <c r="F92" t="n">
         <v>1</v>
       </c>
-      <c r="G92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2972,7 +2898,6 @@
       <c r="F93" t="n">
         <v>0.5</v>
       </c>
-      <c r="G93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2999,7 +2924,6 @@
       <c r="F94" t="n">
         <v>0.5</v>
       </c>
-      <c r="G94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3026,7 +2950,6 @@
       <c r="F95" t="n">
         <v>0.5</v>
       </c>
-      <c r="G95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3053,7 +2976,6 @@
       <c r="F96" t="n">
         <v>0.5</v>
       </c>
-      <c r="G96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3080,7 +3002,6 @@
       <c r="F97" t="n">
         <v>0.5</v>
       </c>
-      <c r="G97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3107,7 +3028,6 @@
       <c r="F98" t="n">
         <v>0.5</v>
       </c>
-      <c r="G98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3134,7 +3054,6 @@
       <c r="F99" t="n">
         <v>0.5</v>
       </c>
-      <c r="G99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3161,7 +3080,6 @@
       <c r="F100" t="n">
         <v>4</v>
       </c>
-      <c r="G100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3188,7 +3106,6 @@
       <c r="F101" t="n">
         <v>0.5</v>
       </c>
-      <c r="G101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3215,7 +3132,6 @@
       <c r="F102" t="n">
         <v>16.5</v>
       </c>
-      <c r="G102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3242,7 +3158,6 @@
       <c r="F103" t="n">
         <v>2</v>
       </c>
-      <c r="G103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3269,7 +3184,6 @@
       <c r="F104" t="n">
         <v>0.5</v>
       </c>
-      <c r="G104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3296,7 +3210,6 @@
       <c r="F105" t="n">
         <v>-89</v>
       </c>
-      <c r="G105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3323,7 +3236,6 @@
       <c r="F106" t="n">
         <v>-1</v>
       </c>
-      <c r="G106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3350,31 +3262,30 @@
       <c r="F107" t="n">
         <v>32</v>
       </c>
-      <c r="G107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>2456</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t>2456</t>
+        </is>
+      </c>
+      <c r="B108" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
+      <c r="C108" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D108" t="n">
+      <c r="D108" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E108" t="n">
+      <c r="E108" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="F108" t="n">
+      <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G108" t="n">
@@ -3406,7 +3317,6 @@
       <c r="F109" t="n">
         <v>0.5</v>
       </c>
-      <c r="G109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3433,7 +3343,6 @@
       <c r="F110" t="n">
         <v>1</v>
       </c>
-      <c r="G110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3460,7 +3369,6 @@
       <c r="F111" t="n">
         <v>0.5</v>
       </c>
-      <c r="G111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3487,7 +3395,6 @@
       <c r="F112" t="n">
         <v>0.5</v>
       </c>
-      <c r="G112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3514,7 +3421,6 @@
       <c r="F113" t="n">
         <v>1</v>
       </c>
-      <c r="G113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3541,7 +3447,6 @@
       <c r="F114" t="n">
         <v>0.5</v>
       </c>
-      <c r="G114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3568,7 +3473,6 @@
       <c r="F115" t="n">
         <v>0.5</v>
       </c>
-      <c r="G115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3595,7 +3499,6 @@
       <c r="F116" t="n">
         <v>0.5</v>
       </c>
-      <c r="G116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3622,7 +3525,6 @@
       <c r="F117" t="n">
         <v>0.5</v>
       </c>
-      <c r="G117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3649,7 +3551,6 @@
       <c r="F118" t="n">
         <v>0.5</v>
       </c>
-      <c r="G118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3676,7 +3577,6 @@
       <c r="F119" t="n">
         <v>1.5</v>
       </c>
-      <c r="G119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3703,7 +3603,6 @@
       <c r="F120" t="n">
         <v>1</v>
       </c>
-      <c r="G120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3730,7 +3629,6 @@
       <c r="F121" t="n">
         <v>0.5</v>
       </c>
-      <c r="G121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3757,7 +3655,6 @@
       <c r="F122" t="n">
         <v>0.5</v>
       </c>
-      <c r="G122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3784,7 +3681,6 @@
       <c r="F123" t="n">
         <v>0.5</v>
       </c>
-      <c r="G123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3811,7 +3707,6 @@
       <c r="F124" t="n">
         <v>1</v>
       </c>
-      <c r="G124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3838,7 +3733,6 @@
       <c r="F125" t="n">
         <v>1.5</v>
       </c>
-      <c r="G125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3865,7 +3759,6 @@
       <c r="F126" t="n">
         <v>1</v>
       </c>
-      <c r="G126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3892,7 +3785,6 @@
       <c r="F127" t="n">
         <v>2.5</v>
       </c>
-      <c r="G127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3919,7 +3811,6 @@
       <c r="F128" t="n">
         <v>0.5</v>
       </c>
-      <c r="G128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3946,7 +3837,6 @@
       <c r="F129" t="n">
         <v>2</v>
       </c>
-      <c r="G129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3973,7 +3863,6 @@
       <c r="F130" t="n">
         <v>1</v>
       </c>
-      <c r="G130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4000,7 +3889,6 @@
       <c r="F131" t="n">
         <v>0.5</v>
       </c>
-      <c r="G131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4027,7 +3915,6 @@
       <c r="F132" t="n">
         <v>0.5</v>
       </c>
-      <c r="G132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4054,7 +3941,6 @@
       <c r="F133" t="n">
         <v>1.5</v>
       </c>
-      <c r="G133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4081,7 +3967,6 @@
       <c r="F134" t="n">
         <v>2</v>
       </c>
-      <c r="G134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4108,7 +3993,6 @@
       <c r="F135" t="n">
         <v>1</v>
       </c>
-      <c r="G135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4135,7 +4019,6 @@
       <c r="F136" t="n">
         <v>1.5</v>
       </c>
-      <c r="G136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4162,7 +4045,6 @@
       <c r="F137" t="n">
         <v>0.5</v>
       </c>
-      <c r="G137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4189,7 +4071,6 @@
       <c r="F138" t="n">
         <v>1.5</v>
       </c>
-      <c r="G138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4216,7 +4097,6 @@
       <c r="F139" t="n">
         <v>1</v>
       </c>
-      <c r="G139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4243,7 +4123,6 @@
       <c r="F140" t="n">
         <v>0.5</v>
       </c>
-      <c r="G140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -4270,7 +4149,6 @@
       <c r="F141" t="n">
         <v>0.5</v>
       </c>
-      <c r="G141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4297,7 +4175,6 @@
       <c r="F142" t="n">
         <v>0.5</v>
       </c>
-      <c r="G142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4324,7 +4201,6 @@
       <c r="F143" t="n">
         <v>1</v>
       </c>
-      <c r="G143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4351,7 +4227,6 @@
       <c r="F144" t="n">
         <v>1.5</v>
       </c>
-      <c r="G144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -4378,7 +4253,6 @@
       <c r="F145" t="n">
         <v>5.5</v>
       </c>
-      <c r="G145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4405,7 +4279,6 @@
       <c r="F146" t="n">
         <v>1</v>
       </c>
-      <c r="G146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -4432,7 +4305,6 @@
       <c r="F147" t="n">
         <v>0.5</v>
       </c>
-      <c r="G147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -4459,7 +4331,6 @@
       <c r="F148" t="n">
         <v>0.5</v>
       </c>
-      <c r="G148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -4486,7 +4357,6 @@
       <c r="F149" t="n">
         <v>1</v>
       </c>
-      <c r="G149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -4513,7 +4383,6 @@
       <c r="F150" t="n">
         <v>1</v>
       </c>
-      <c r="G150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -4540,7 +4409,6 @@
       <c r="F151" t="n">
         <v>1</v>
       </c>
-      <c r="G151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -4567,7 +4435,6 @@
       <c r="F152" t="n">
         <v>1</v>
       </c>
-      <c r="G152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -4594,7 +4461,6 @@
       <c r="F153" t="n">
         <v>9</v>
       </c>
-      <c r="G153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -4621,7 +4487,6 @@
       <c r="F154" t="n">
         <v>0.5</v>
       </c>
-      <c r="G154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -4648,7 +4513,6 @@
       <c r="F155" t="n">
         <v>3</v>
       </c>
-      <c r="G155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -4675,7 +4539,6 @@
       <c r="F156" t="n">
         <v>-94</v>
       </c>
-      <c r="G156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -4702,7 +4565,6 @@
       <c r="F157" t="n">
         <v>-33</v>
       </c>
-      <c r="G157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -4729,31 +4591,30 @@
       <c r="F158" t="n">
         <v>61.5</v>
       </c>
-      <c r="G158" t="inlineStr"/>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>2456</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
+      <c r="A159" s="2" t="inlineStr">
+        <is>
+          <t>2456</t>
+        </is>
+      </c>
+      <c r="B159" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D159" t="n">
+      <c r="C159" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D159" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="E159" t="n">
+      <c r="E159" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="F159" t="n">
+      <c r="F159" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G159" t="n">
@@ -4785,31 +4646,30 @@
       <c r="F160" t="n">
         <v>120</v>
       </c>
-      <c r="G160" t="inlineStr"/>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr">
+      <c r="A161" s="2" t="inlineStr">
         <is>
           <t>2496</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr">
+      <c r="B161" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C161" t="inlineStr">
+      <c r="C161" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D161" t="n">
+      <c r="D161" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E161" t="n">
-        <v>0</v>
-      </c>
-      <c r="F161" t="n">
+      <c r="E161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F161" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G161" t="n">
@@ -4841,7 +4701,6 @@
       <c r="F162" t="n">
         <v>135</v>
       </c>
-      <c r="G162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -4868,31 +4727,30 @@
       <c r="F163" t="n">
         <v>9</v>
       </c>
-      <c r="G163" t="inlineStr"/>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
+      <c r="A164" s="2" t="inlineStr">
         <is>
           <t>2496</t>
         </is>
       </c>
-      <c r="B164" t="inlineStr">
+      <c r="B164" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C164" t="inlineStr">
+      <c r="C164" s="2" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="D164" t="n">
-        <v>0</v>
-      </c>
-      <c r="E164" t="n">
+      <c r="D164" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E164" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F164" t="n">
+      <c r="F164" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G164" t="n">
@@ -4924,7 +4782,6 @@
       <c r="F165" t="n">
         <v>90</v>
       </c>
-      <c r="G165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -4951,31 +4808,30 @@
       <c r="F166" t="n">
         <v>62</v>
       </c>
-      <c r="G166" t="inlineStr"/>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
+      <c r="A167" s="2" t="inlineStr">
         <is>
           <t>2496</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
+      <c r="B167" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C167" t="inlineStr">
+      <c r="C167" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D167" t="n">
+      <c r="D167" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E167" t="n">
+      <c r="E167" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F167" t="n">
+      <c r="F167" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G167" t="n">
@@ -5036,7 +4892,6 @@
       <c r="F169" t="n">
         <v>-48</v>
       </c>
-      <c r="G169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -5092,7 +4947,6 @@
       <c r="F171" t="n">
         <v>-60</v>
       </c>
-      <c r="G171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -5119,31 +4973,30 @@
       <c r="F172" t="n">
         <v>-4</v>
       </c>
-      <c r="G172" t="inlineStr"/>
     </row>
     <row r="173">
-      <c r="A173" t="inlineStr">
+      <c r="A173" s="2" t="inlineStr">
         <is>
           <t>5776</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
+      <c r="B173" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C173" t="inlineStr">
+      <c r="C173" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D173" t="n">
+      <c r="D173" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E173" t="n">
-        <v>0</v>
-      </c>
-      <c r="F173" t="n">
+      <c r="E173" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F173" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G173" t="n">
@@ -5175,7 +5028,6 @@
       <c r="F174" t="n">
         <v>-12</v>
       </c>
-      <c r="G174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -5202,7 +5054,6 @@
       <c r="F175" t="n">
         <v>-80</v>
       </c>
-      <c r="G175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -5229,31 +5080,30 @@
       <c r="F176" t="n">
         <v>104</v>
       </c>
-      <c r="G176" t="inlineStr"/>
     </row>
     <row r="177">
-      <c r="A177" t="inlineStr">
+      <c r="A177" s="2" t="inlineStr">
         <is>
           <t>5788</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
+      <c r="B177" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C177" t="inlineStr">
+      <c r="C177" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D177" t="n">
+      <c r="D177" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E177" t="n">
+      <c r="E177" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="F177" t="n">
+      <c r="F177" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G177" t="n">
@@ -5285,7 +5135,6 @@
       <c r="F178" t="n">
         <v>0.5</v>
       </c>
-      <c r="G178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -5312,7 +5161,6 @@
       <c r="F179" t="n">
         <v>30</v>
       </c>
-      <c r="G179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -5339,7 +5187,6 @@
       <c r="F180" t="n">
         <v>-16</v>
       </c>
-      <c r="G180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -5366,7 +5213,6 @@
       <c r="F181" t="n">
         <v>17</v>
       </c>
-      <c r="G181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -5393,7 +5239,6 @@
       <c r="F182" t="n">
         <v>22</v>
       </c>
-      <c r="G182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -5420,7 +5265,6 @@
       <c r="F183" t="n">
         <v>-52.5</v>
       </c>
-      <c r="G183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -5476,7 +5320,6 @@
       <c r="F185" t="n">
         <v>-4</v>
       </c>
-      <c r="G185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -5503,31 +5346,30 @@
       <c r="F186" t="n">
         <v>144</v>
       </c>
-      <c r="G186" t="inlineStr"/>
     </row>
     <row r="187">
-      <c r="A187" t="inlineStr">
+      <c r="A187" s="2" t="inlineStr">
         <is>
           <t>5788</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
+      <c r="B187" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C187" t="inlineStr">
+      <c r="C187" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D187" t="n">
+      <c r="D187" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E187" t="n">
+      <c r="E187" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="F187" t="n">
+      <c r="F187" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G187" t="n">
@@ -5559,7 +5401,6 @@
       <c r="F188" t="n">
         <v>-14</v>
       </c>
-      <c r="G188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -5586,7 +5427,6 @@
       <c r="F189" t="n">
         <v>0</v>
       </c>
-      <c r="G189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -5613,7 +5453,6 @@
       <c r="F190" t="n">
         <v>4</v>
       </c>
-      <c r="G190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -5640,7 +5479,6 @@
       <c r="F191" t="n">
         <v>-65.5</v>
       </c>
-      <c r="G191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -5667,31 +5505,30 @@
       <c r="F192" t="n">
         <v>131.5</v>
       </c>
-      <c r="G192" t="inlineStr"/>
     </row>
     <row r="193">
-      <c r="A193" t="inlineStr">
+      <c r="A193" s="2" t="inlineStr">
         <is>
           <t>5788</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr">
+      <c r="B193" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C193" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D193" t="n">
+      <c r="C193" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D193" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E193" t="n">
-        <v>0</v>
-      </c>
-      <c r="F193" t="n">
+      <c r="E193" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F193" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G193" t="n">
@@ -5723,7 +5560,6 @@
       <c r="F194" t="n">
         <v>-16</v>
       </c>
-      <c r="G194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -5750,7 +5586,6 @@
       <c r="F195" t="n">
         <v>-36</v>
       </c>
-      <c r="G195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -5777,7 +5612,6 @@
       <c r="F196" t="n">
         <v>13</v>
       </c>
-      <c r="G196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -5804,7 +5638,6 @@
       <c r="F197" t="n">
         <v>2</v>
       </c>
-      <c r="G197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -5831,7 +5664,6 @@
       <c r="F198" t="n">
         <v>28</v>
       </c>
-      <c r="G198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -5858,31 +5690,30 @@
       <c r="F199" t="n">
         <v>9</v>
       </c>
-      <c r="G199" t="inlineStr"/>
     </row>
     <row r="200">
-      <c r="A200" t="inlineStr">
+      <c r="A200" s="2" t="inlineStr">
         <is>
           <t>5829</t>
         </is>
       </c>
-      <c r="B200" t="inlineStr">
+      <c r="B200" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C200" t="inlineStr">
+      <c r="C200" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D200" t="n">
+      <c r="D200" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E200" t="n">
+      <c r="E200" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="F200" t="n">
+      <c r="F200" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G200" t="n">
@@ -5914,7 +5745,6 @@
       <c r="F201" t="n">
         <v>-16</v>
       </c>
-      <c r="G201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -5941,7 +5771,6 @@
       <c r="F202" t="n">
         <v>45</v>
       </c>
-      <c r="G202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -5968,7 +5797,6 @@
       <c r="F203" t="n">
         <v>1</v>
       </c>
-      <c r="G203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -5995,31 +5823,30 @@
       <c r="F204" t="n">
         <v>10</v>
       </c>
-      <c r="G204" t="inlineStr"/>
     </row>
     <row r="205">
-      <c r="A205" t="inlineStr">
+      <c r="A205" s="2" t="inlineStr">
         <is>
           <t>5829</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr">
+      <c r="B205" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C205" t="inlineStr">
+      <c r="C205" s="2" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="D205" t="n">
+      <c r="D205" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="E205" t="n">
+      <c r="E205" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="F205" t="n">
+      <c r="F205" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G205" t="n">
@@ -6051,7 +5878,6 @@
       <c r="F206" t="n">
         <v>-20</v>
       </c>
-      <c r="G206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -6078,7 +5904,6 @@
       <c r="F207" t="n">
         <v>12.5</v>
       </c>
-      <c r="G207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -6105,7 +5930,6 @@
       <c r="F208" t="n">
         <v>44.5</v>
       </c>
-      <c r="G208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -6132,31 +5956,30 @@
       <c r="F209" t="n">
         <v>7</v>
       </c>
-      <c r="G209" t="inlineStr"/>
     </row>
     <row r="210">
-      <c r="A210" t="inlineStr">
+      <c r="A210" s="2" t="inlineStr">
         <is>
           <t>5829</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr">
+      <c r="B210" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C210" t="inlineStr">
+      <c r="C210" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D210" t="n">
+      <c r="D210" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E210" t="n">
-        <v>0</v>
-      </c>
-      <c r="F210" t="n">
+      <c r="E210" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F210" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G210" t="n">
@@ -6188,7 +6011,6 @@
       <c r="F211" t="n">
         <v>-16</v>
       </c>
-      <c r="G211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -6215,7 +6037,6 @@
       <c r="F212" t="n">
         <v>-24</v>
       </c>
-      <c r="G212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -6242,7 +6063,6 @@
       <c r="F213" t="n">
         <v>-50.5</v>
       </c>
-      <c r="G213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -6269,7 +6089,6 @@
       <c r="F214" t="n">
         <v>-13</v>
       </c>
-      <c r="G214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -6296,7 +6115,6 @@
       <c r="F215" t="n">
         <v>48.5</v>
       </c>
-      <c r="G215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -6323,7 +6141,6 @@
       <c r="F216" t="n">
         <v>48</v>
       </c>
-      <c r="G216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -6350,31 +6167,30 @@
       <c r="F217" t="n">
         <v>7</v>
       </c>
-      <c r="G217" t="inlineStr"/>
     </row>
     <row r="218">
-      <c r="A218" t="inlineStr">
+      <c r="A218" s="2" t="inlineStr">
         <is>
           <t>5829</t>
         </is>
       </c>
-      <c r="B218" t="inlineStr">
+      <c r="B218" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D218" t="n">
+      <c r="C218" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D218" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E218" t="n">
-        <v>0</v>
-      </c>
-      <c r="F218" t="n">
+      <c r="E218" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F218" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G218" t="n">
@@ -6406,7 +6222,6 @@
       <c r="F219" t="n">
         <v>-48</v>
       </c>
-      <c r="G219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -6433,7 +6248,6 @@
       <c r="F220" t="n">
         <v>-64</v>
       </c>
-      <c r="G220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -6460,7 +6274,6 @@
       <c r="F221" t="n">
         <v>40</v>
       </c>
-      <c r="G221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -6487,31 +6300,30 @@
       <c r="F222" t="n">
         <v>16</v>
       </c>
-      <c r="G222" t="inlineStr"/>
     </row>
     <row r="223">
-      <c r="A223" t="inlineStr">
+      <c r="A223" s="2" t="inlineStr">
         <is>
           <t>5972</t>
         </is>
       </c>
-      <c r="B223" t="inlineStr">
+      <c r="B223" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C223" t="inlineStr">
+      <c r="C223" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D223" t="n">
+      <c r="D223" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E223" t="n">
+      <c r="E223" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F223" t="n">
+      <c r="F223" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G223" t="n">
@@ -6543,7 +6355,6 @@
       <c r="F224" t="n">
         <v>8</v>
       </c>
-      <c r="G224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -6570,7 +6381,6 @@
       <c r="F225" t="n">
         <v>-48</v>
       </c>
-      <c r="G225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -6597,7 +6407,6 @@
       <c r="F226" t="n">
         <v>-32</v>
       </c>
-      <c r="G226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -6624,7 +6433,6 @@
       <c r="F227" t="n">
         <v>6</v>
       </c>
-      <c r="G227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -6651,31 +6459,30 @@
       <c r="F228" t="n">
         <v>130</v>
       </c>
-      <c r="G228" t="inlineStr"/>
     </row>
     <row r="229">
-      <c r="A229" t="inlineStr">
+      <c r="A229" s="2" t="inlineStr">
         <is>
           <t>5972</t>
         </is>
       </c>
-      <c r="B229" t="inlineStr">
+      <c r="B229" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C229" t="inlineStr">
+      <c r="C229" s="2" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="D229" t="n">
-        <v>0</v>
-      </c>
-      <c r="E229" t="n">
+      <c r="D229" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E229" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F229" t="n">
+      <c r="F229" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G229" t="n">
@@ -6707,7 +6514,6 @@
       <c r="F230" t="n">
         <v>-60</v>
       </c>
-      <c r="G230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -6734,7 +6540,6 @@
       <c r="F231" t="n">
         <v>4</v>
       </c>
-      <c r="G231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -6761,7 +6566,6 @@
       <c r="F232" t="n">
         <v>16</v>
       </c>
-      <c r="G232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -6788,7 +6592,6 @@
       <c r="F233" t="n">
         <v>-36</v>
       </c>
-      <c r="G233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -6815,31 +6618,30 @@
       <c r="F234" t="n">
         <v>84</v>
       </c>
-      <c r="G234" t="inlineStr"/>
     </row>
     <row r="235">
-      <c r="A235" t="inlineStr">
+      <c r="A235" s="2" t="inlineStr">
         <is>
           <t>5972</t>
         </is>
       </c>
-      <c r="B235" t="inlineStr">
+      <c r="B235" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C235" t="inlineStr">
+      <c r="C235" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D235" t="n">
+      <c r="D235" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E235" t="n">
+      <c r="E235" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="F235" t="n">
+      <c r="F235" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G235" t="n">
@@ -6871,7 +6673,6 @@
       <c r="F236" t="n">
         <v>8</v>
       </c>
-      <c r="G236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -6898,7 +6699,6 @@
       <c r="F237" t="n">
         <v>16</v>
       </c>
-      <c r="G237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -6925,7 +6725,6 @@
       <c r="F238" t="n">
         <v>40</v>
       </c>
-      <c r="G238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -6952,7 +6751,6 @@
       <c r="F239" t="n">
         <v>24</v>
       </c>
-      <c r="G239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -6979,7 +6777,6 @@
       <c r="F240" t="n">
         <v>-48</v>
       </c>
-      <c r="G240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -7006,7 +6803,6 @@
       <c r="F241" t="n">
         <v>8</v>
       </c>
-      <c r="G241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -7033,7 +6829,6 @@
       <c r="F242" t="n">
         <v>-8</v>
       </c>
-      <c r="G242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -7060,7 +6855,6 @@
       <c r="F243" t="n">
         <v>-64</v>
       </c>
-      <c r="G243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -7087,7 +6881,6 @@
       <c r="F244" t="n">
         <v>-48</v>
       </c>
-      <c r="G244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -7114,31 +6907,30 @@
       <c r="F245" t="n">
         <v>32</v>
       </c>
-      <c r="G245" t="inlineStr"/>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr">
+      <c r="A246" s="2" t="inlineStr">
         <is>
           <t>5972</t>
         </is>
       </c>
-      <c r="B246" t="inlineStr">
+      <c r="B246" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C246" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D246" t="n">
+      <c r="C246" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D246" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="E246" t="n">
+      <c r="E246" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="F246" t="n">
+      <c r="F246" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G246" t="n">
@@ -7170,7 +6962,6 @@
       <c r="F247" t="n">
         <v>13.5</v>
       </c>
-      <c r="G247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -7197,7 +6988,6 @@
       <c r="F248" t="n">
         <v>-16</v>
       </c>
-      <c r="G248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -7224,7 +7014,6 @@
       <c r="F249" t="n">
         <v>-0.5</v>
       </c>
-      <c r="G249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -7251,7 +7040,6 @@
       <c r="F250" t="n">
         <v>13</v>
       </c>
-      <c r="G250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -7278,7 +7066,6 @@
       <c r="F251" t="n">
         <v>9.5</v>
       </c>
-      <c r="G251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -7305,7 +7092,6 @@
       <c r="F252" t="n">
         <v>1.5</v>
       </c>
-      <c r="G252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -7332,7 +7118,6 @@
       <c r="F253" t="n">
         <v>1.5</v>
       </c>
-      <c r="G253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -7359,7 +7144,6 @@
       <c r="F254" t="n">
         <v>-2</v>
       </c>
-      <c r="G254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -7386,7 +7170,6 @@
       <c r="F255" t="n">
         <v>-32</v>
       </c>
-      <c r="G255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -7413,7 +7196,6 @@
       <c r="F256" t="n">
         <v>1</v>
       </c>
-      <c r="G256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -7440,7 +7222,6 @@
       <c r="F257" t="n">
         <v>-46</v>
       </c>
-      <c r="G257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -7467,7 +7248,6 @@
       <c r="F258" t="n">
         <v>-36.5</v>
       </c>
-      <c r="G258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -7494,31 +7274,30 @@
       <c r="F259" t="n">
         <v>9.5</v>
       </c>
-      <c r="G259" t="inlineStr"/>
     </row>
     <row r="260">
-      <c r="A260" t="inlineStr">
+      <c r="A260" s="2" t="inlineStr">
         <is>
           <t>5977</t>
         </is>
       </c>
-      <c r="B260" t="inlineStr">
+      <c r="B260" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C260" t="inlineStr">
+      <c r="C260" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D260" t="n">
-        <v>0</v>
-      </c>
-      <c r="E260" t="n">
+      <c r="D260" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E260" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="F260" t="n">
+      <c r="F260" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G260" t="n">
@@ -7550,7 +7329,6 @@
       <c r="F261" t="n">
         <v>-16</v>
       </c>
-      <c r="G261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -7577,7 +7355,6 @@
       <c r="F262" t="n">
         <v>1</v>
       </c>
-      <c r="G262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -7604,7 +7381,6 @@
       <c r="F263" t="n">
         <v>32.5</v>
       </c>
-      <c r="G263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -7631,7 +7407,6 @@
       <c r="F264" t="n">
         <v>1</v>
       </c>
-      <c r="G264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -7658,7 +7433,6 @@
       <c r="F265" t="n">
         <v>4</v>
       </c>
-      <c r="G265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -7685,7 +7459,6 @@
       <c r="F266" t="n">
         <v>1</v>
       </c>
-      <c r="G266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -7712,7 +7485,6 @@
       <c r="F267" t="n">
         <v>22</v>
       </c>
-      <c r="G267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -7739,7 +7511,6 @@
       <c r="F268" t="n">
         <v>3.5</v>
       </c>
-      <c r="G268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -7766,7 +7537,6 @@
       <c r="F269" t="n">
         <v>10.5</v>
       </c>
-      <c r="G269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -7793,7 +7563,6 @@
       <c r="F270" t="n">
         <v>1.5</v>
       </c>
-      <c r="G270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -7820,7 +7589,6 @@
       <c r="F271" t="n">
         <v>5.5</v>
       </c>
-      <c r="G271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -7847,7 +7615,6 @@
       <c r="F272" t="n">
         <v>1</v>
       </c>
-      <c r="G272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -7874,7 +7641,6 @@
       <c r="F273" t="n">
         <v>0.5</v>
       </c>
-      <c r="G273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -7901,7 +7667,6 @@
       <c r="F274" t="n">
         <v>5</v>
       </c>
-      <c r="G274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -7928,7 +7693,6 @@
       <c r="F275" t="n">
         <v>-73.5</v>
       </c>
-      <c r="G275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -7955,7 +7719,6 @@
       <c r="F276" t="n">
         <v>-16</v>
       </c>
-      <c r="G276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -8011,7 +7774,6 @@
       <c r="F278" t="n">
         <v>8</v>
       </c>
-      <c r="G278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -8038,7 +7800,6 @@
       <c r="F279" t="n">
         <v>3.5</v>
       </c>
-      <c r="G279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -8065,7 +7826,6 @@
       <c r="F280" t="n">
         <v>1</v>
       </c>
-      <c r="G280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -8092,7 +7852,6 @@
       <c r="F281" t="n">
         <v>-4</v>
       </c>
-      <c r="G281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -8119,7 +7878,6 @@
       <c r="F282" t="n">
         <v>-6</v>
       </c>
-      <c r="G282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -8146,7 +7904,6 @@
       <c r="F283" t="n">
         <v>3.5</v>
       </c>
-      <c r="G283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -8173,7 +7930,6 @@
       <c r="F284" t="n">
         <v>1.5</v>
       </c>
-      <c r="G284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -8200,7 +7956,6 @@
       <c r="F285" t="n">
         <v>2.5</v>
       </c>
-      <c r="G285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -8227,7 +7982,6 @@
       <c r="F286" t="n">
         <v>8</v>
       </c>
-      <c r="G286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -8254,7 +8008,6 @@
       <c r="F287" t="n">
         <v>21.5</v>
       </c>
-      <c r="G287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -8281,7 +8034,6 @@
       <c r="F288" t="n">
         <v>1</v>
       </c>
-      <c r="G288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -8308,7 +8060,6 @@
       <c r="F289" t="n">
         <v>-48</v>
       </c>
-      <c r="G289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -8335,7 +8086,6 @@
       <c r="F290" t="n">
         <v>-91</v>
       </c>
-      <c r="G290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -8362,31 +8112,30 @@
       <c r="F291" t="n">
         <v>2.5</v>
       </c>
-      <c r="G291" t="inlineStr"/>
     </row>
     <row r="292">
-      <c r="A292" t="inlineStr">
+      <c r="A292" s="2" t="inlineStr">
         <is>
           <t>5977</t>
         </is>
       </c>
-      <c r="B292" t="inlineStr">
+      <c r="B292" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C292" t="inlineStr">
+      <c r="C292" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D292" t="n">
+      <c r="D292" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E292" t="n">
+      <c r="E292" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F292" t="n">
+      <c r="F292" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G292" t="n">
@@ -8418,7 +8167,6 @@
       <c r="F293" t="n">
         <v>17</v>
       </c>
-      <c r="G293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -8445,7 +8193,6 @@
       <c r="F294" t="n">
         <v>-16</v>
       </c>
-      <c r="G294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -8472,7 +8219,6 @@
       <c r="F295" t="n">
         <v>4.5</v>
       </c>
-      <c r="G295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -8499,7 +8245,6 @@
       <c r="F296" t="n">
         <v>2</v>
       </c>
-      <c r="G296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -8526,7 +8271,6 @@
       <c r="F297" t="n">
         <v>0.5</v>
       </c>
-      <c r="G297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -8553,7 +8297,6 @@
       <c r="F298" t="n">
         <v>23.5</v>
       </c>
-      <c r="G298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -8580,7 +8323,6 @@
       <c r="F299" t="n">
         <v>2</v>
       </c>
-      <c r="G299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -8607,7 +8349,6 @@
       <c r="F300" t="n">
         <v>1</v>
       </c>
-      <c r="G300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -8634,7 +8375,6 @@
       <c r="F301" t="n">
         <v>2</v>
       </c>
-      <c r="G301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -8661,7 +8401,6 @@
       <c r="F302" t="n">
         <v>1.5</v>
       </c>
-      <c r="G302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -8688,7 +8427,6 @@
       <c r="F303" t="n">
         <v>0.5</v>
       </c>
-      <c r="G303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -8715,7 +8453,6 @@
       <c r="F304" t="n">
         <v>1</v>
       </c>
-      <c r="G304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -8742,7 +8479,6 @@
       <c r="F305" t="n">
         <v>1</v>
       </c>
-      <c r="G305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -8769,7 +8505,6 @@
       <c r="F306" t="n">
         <v>-37</v>
       </c>
-      <c r="G306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -8796,7 +8531,6 @@
       <c r="F307" t="n">
         <v>-45</v>
       </c>
-      <c r="G307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -8823,7 +8557,6 @@
       <c r="F308" t="n">
         <v>-39.5</v>
       </c>
-      <c r="G308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -8850,31 +8583,30 @@
       <c r="F309" t="n">
         <v>1</v>
       </c>
-      <c r="G309" t="inlineStr"/>
     </row>
     <row r="310">
-      <c r="A310" t="inlineStr">
+      <c r="A310" s="2" t="inlineStr">
         <is>
           <t>5977</t>
         </is>
       </c>
-      <c r="B310" t="inlineStr">
+      <c r="B310" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C310" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D310" t="n">
-        <v>0</v>
-      </c>
-      <c r="E310" t="n">
+      <c r="C310" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D310" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E310" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="F310" t="n">
+      <c r="F310" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G310" t="n">
@@ -8906,7 +8638,6 @@
       <c r="F311" t="n">
         <v>1</v>
       </c>
-      <c r="G311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -8933,7 +8664,6 @@
       <c r="F312" t="n">
         <v>-54</v>
       </c>
-      <c r="G312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -8960,7 +8690,6 @@
       <c r="F313" t="n">
         <v>24</v>
       </c>
-      <c r="G313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -8987,7 +8716,6 @@
       <c r="F314" t="n">
         <v>-21</v>
       </c>
-      <c r="G314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -9014,31 +8742,30 @@
       <c r="F315" t="n">
         <v>2</v>
       </c>
-      <c r="G315" t="inlineStr"/>
     </row>
     <row r="316">
-      <c r="A316" t="inlineStr">
+      <c r="A316" s="2" t="inlineStr">
         <is>
           <t>6093</t>
         </is>
       </c>
-      <c r="B316" t="inlineStr">
+      <c r="B316" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C316" t="inlineStr">
+      <c r="C316" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D316" t="n">
+      <c r="D316" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E316" t="n">
+      <c r="E316" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="F316" t="n">
+      <c r="F316" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G316" t="n">
@@ -9070,7 +8797,6 @@
       <c r="F317" t="n">
         <v>27</v>
       </c>
-      <c r="G317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -9097,7 +8823,6 @@
       <c r="F318" t="n">
         <v>-8</v>
       </c>
-      <c r="G318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -9124,7 +8849,6 @@
       <c r="F319" t="n">
         <v>3</v>
       </c>
-      <c r="G319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -9180,7 +8904,6 @@
       <c r="F321" t="n">
         <v>-34</v>
       </c>
-      <c r="G321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -9207,7 +8930,6 @@
       <c r="F322" t="n">
         <v>-4</v>
       </c>
-      <c r="G322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -9234,31 +8956,30 @@
       <c r="F323" t="n">
         <v>6</v>
       </c>
-      <c r="G323" t="inlineStr"/>
     </row>
     <row r="324">
-      <c r="A324" t="inlineStr">
+      <c r="A324" s="2" t="inlineStr">
         <is>
           <t>6093</t>
         </is>
       </c>
-      <c r="B324" t="inlineStr">
+      <c r="B324" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C324" t="inlineStr">
+      <c r="C324" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D324" t="n">
+      <c r="D324" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E324" t="n">
+      <c r="E324" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="F324" t="n">
+      <c r="F324" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G324" t="n">
@@ -9290,7 +9011,6 @@
       <c r="F325" t="n">
         <v>3</v>
       </c>
-      <c r="G325" t="inlineStr"/>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -9317,7 +9037,6 @@
       <c r="F326" t="n">
         <v>-10</v>
       </c>
-      <c r="G326" t="inlineStr"/>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -9344,7 +9063,6 @@
       <c r="F327" t="n">
         <v>14</v>
       </c>
-      <c r="G327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -9371,7 +9089,6 @@
       <c r="F328" t="n">
         <v>-10</v>
       </c>
-      <c r="G328" t="inlineStr"/>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -9398,31 +9115,30 @@
       <c r="F329" t="n">
         <v>11</v>
       </c>
-      <c r="G329" t="inlineStr"/>
     </row>
     <row r="330">
-      <c r="A330" t="inlineStr">
+      <c r="A330" s="2" t="inlineStr">
         <is>
           <t>6093</t>
         </is>
       </c>
-      <c r="B330" t="inlineStr">
+      <c r="B330" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C330" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D330" t="n">
+      <c r="C330" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D330" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E330" t="n">
-        <v>0</v>
-      </c>
-      <c r="F330" t="n">
+      <c r="E330" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F330" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G330" t="n">
@@ -9454,7 +9170,6 @@
       <c r="F331" t="n">
         <v>15</v>
       </c>
-      <c r="G331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -9481,7 +9196,6 @@
       <c r="F332" t="n">
         <v>1</v>
       </c>
-      <c r="G332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -9508,7 +9222,6 @@
       <c r="F333" t="n">
         <v>-139.5</v>
       </c>
-      <c r="G333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -9535,31 +9248,30 @@
       <c r="F334" t="n">
         <v>43.5</v>
       </c>
-      <c r="G334" t="inlineStr"/>
     </row>
     <row r="335">
-      <c r="A335" t="inlineStr">
+      <c r="A335" s="2" t="inlineStr">
         <is>
           <t>6139</t>
         </is>
       </c>
-      <c r="B335" t="inlineStr">
+      <c r="B335" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C335" t="inlineStr">
+      <c r="C335" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D335" t="n">
+      <c r="D335" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E335" t="n">
+      <c r="E335" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="F335" t="n">
+      <c r="F335" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G335" t="n">
@@ -9591,7 +9303,6 @@
       <c r="F336" t="n">
         <v>34.5</v>
       </c>
-      <c r="G336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -9618,7 +9329,6 @@
       <c r="F337" t="n">
         <v>2</v>
       </c>
-      <c r="G337" t="inlineStr"/>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -9645,7 +9355,6 @@
       <c r="F338" t="n">
         <v>-80</v>
       </c>
-      <c r="G338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -9701,7 +9410,6 @@
       <c r="F340" t="n">
         <v>14.5</v>
       </c>
-      <c r="G340" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -9728,7 +9436,6 @@
       <c r="F341" t="n">
         <v>-100</v>
       </c>
-      <c r="G341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -9755,31 +9462,30 @@
       <c r="F342" t="n">
         <v>121.5</v>
       </c>
-      <c r="G342" t="inlineStr"/>
     </row>
     <row r="343">
-      <c r="A343" t="inlineStr">
+      <c r="A343" s="2" t="inlineStr">
         <is>
           <t>6139</t>
         </is>
       </c>
-      <c r="B343" t="inlineStr">
+      <c r="B343" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C343" t="inlineStr">
+      <c r="C343" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D343" t="n">
+      <c r="D343" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E343" t="n">
+      <c r="E343" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F343" t="n">
+      <c r="F343" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G343" t="n">
@@ -9811,7 +9517,6 @@
       <c r="F344" t="n">
         <v>0.5</v>
       </c>
-      <c r="G344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -9838,7 +9543,6 @@
       <c r="F345" t="n">
         <v>5</v>
       </c>
-      <c r="G345" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -9865,7 +9569,6 @@
       <c r="F346" t="n">
         <v>-144</v>
       </c>
-      <c r="G346" t="inlineStr"/>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -9892,31 +9595,30 @@
       <c r="F347" t="n">
         <v>94.5</v>
       </c>
-      <c r="G347" t="inlineStr"/>
     </row>
     <row r="348">
-      <c r="A348" t="inlineStr">
+      <c r="A348" s="2" t="inlineStr">
         <is>
           <t>6139</t>
         </is>
       </c>
-      <c r="B348" t="inlineStr">
+      <c r="B348" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C348" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D348" t="n">
+      <c r="C348" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D348" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E348" t="n">
+      <c r="E348" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="F348" t="n">
+      <c r="F348" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G348" t="n">
@@ -9924,28 +9626,28 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" t="inlineStr">
+      <c r="A349" s="2" t="inlineStr">
         <is>
           <t>6141</t>
         </is>
       </c>
-      <c r="B349" t="inlineStr">
+      <c r="B349" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C349" t="inlineStr">
+      <c r="C349" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D349" t="n">
+      <c r="D349" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E349" t="n">
-        <v>0</v>
-      </c>
-      <c r="F349" t="n">
+      <c r="E349" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F349" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G349" t="n">
@@ -9977,7 +9679,6 @@
       <c r="F350" t="n">
         <v>82.5</v>
       </c>
-      <c r="G350" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -10004,7 +9705,6 @@
       <c r="F351" t="n">
         <v>4</v>
       </c>
-      <c r="G351" t="inlineStr"/>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -10031,7 +9731,6 @@
       <c r="F352" t="n">
         <v>8</v>
       </c>
-      <c r="G352" t="inlineStr"/>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -10058,7 +9757,6 @@
       <c r="F353" t="n">
         <v>-8</v>
       </c>
-      <c r="G353" t="inlineStr"/>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -10085,7 +9783,6 @@
       <c r="F354" t="n">
         <v>-160</v>
       </c>
-      <c r="G354" t="inlineStr"/>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -10112,31 +9809,30 @@
       <c r="F355" t="n">
         <v>9.5</v>
       </c>
-      <c r="G355" t="inlineStr"/>
     </row>
     <row r="356">
-      <c r="A356" t="inlineStr">
+      <c r="A356" s="2" t="inlineStr">
         <is>
           <t>6180</t>
         </is>
       </c>
-      <c r="B356" t="inlineStr">
+      <c r="B356" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C356" t="inlineStr">
+      <c r="C356" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D356" t="n">
-        <v>0</v>
-      </c>
-      <c r="E356" t="n">
+      <c r="D356" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E356" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="F356" t="n">
+      <c r="F356" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G356" t="n">
@@ -10168,7 +9864,6 @@
       <c r="F357" t="n">
         <v>19</v>
       </c>
-      <c r="G357" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -10195,7 +9890,6 @@
       <c r="F358" t="n">
         <v>21</v>
       </c>
-      <c r="G358" t="inlineStr"/>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -10222,7 +9916,6 @@
       <c r="F359" t="n">
         <v>-16</v>
       </c>
-      <c r="G359" t="inlineStr"/>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -10249,7 +9942,6 @@
       <c r="F360" t="n">
         <v>-25</v>
       </c>
-      <c r="G360" t="inlineStr"/>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -10305,7 +9997,6 @@
       <c r="F362" t="n">
         <v>135.5</v>
       </c>
-      <c r="G362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -10332,7 +10023,6 @@
       <c r="F363" t="n">
         <v>3</v>
       </c>
-      <c r="G363" t="inlineStr"/>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -10359,7 +10049,6 @@
       <c r="F364" t="n">
         <v>-4</v>
       </c>
-      <c r="G364" t="inlineStr"/>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -10386,7 +10075,6 @@
       <c r="F365" t="n">
         <v>-101</v>
       </c>
-      <c r="G365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -10413,31 +10101,30 @@
       <c r="F366" t="n">
         <v>10.5</v>
       </c>
-      <c r="G366" t="inlineStr"/>
     </row>
     <row r="367">
-      <c r="A367" t="inlineStr">
+      <c r="A367" s="2" t="inlineStr">
         <is>
           <t>6180</t>
         </is>
       </c>
-      <c r="B367" t="inlineStr">
+      <c r="B367" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C367" t="inlineStr">
+      <c r="C367" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D367" t="n">
+      <c r="D367" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="E367" t="n">
+      <c r="E367" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F367" t="n">
+      <c r="F367" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G367" t="n">
@@ -10469,7 +10156,6 @@
       <c r="F368" t="n">
         <v>9</v>
       </c>
-      <c r="G368" t="inlineStr"/>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -10496,7 +10182,6 @@
       <c r="F369" t="n">
         <v>9</v>
       </c>
-      <c r="G369" t="inlineStr"/>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -10523,7 +10208,6 @@
       <c r="F370" t="n">
         <v>-20</v>
       </c>
-      <c r="G370" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -10550,7 +10234,6 @@
       <c r="F371" t="n">
         <v>-160</v>
       </c>
-      <c r="G371" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -10577,31 +10260,30 @@
       <c r="F372" t="n">
         <v>2</v>
       </c>
-      <c r="G372" t="inlineStr"/>
     </row>
     <row r="373">
-      <c r="A373" t="inlineStr">
+      <c r="A373" s="2" t="inlineStr">
         <is>
           <t>6180</t>
         </is>
       </c>
-      <c r="B373" t="inlineStr">
+      <c r="B373" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C373" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D373" t="n">
-        <v>0</v>
-      </c>
-      <c r="E373" t="n">
+      <c r="C373" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D373" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E373" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="F373" t="n">
+      <c r="F373" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G373" t="n">
@@ -10633,7 +10315,6 @@
       <c r="F374" t="n">
         <v>-19</v>
       </c>
-      <c r="G374" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -10660,7 +10341,6 @@
       <c r="F375" t="n">
         <v>28</v>
       </c>
-      <c r="G375" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -10687,7 +10367,6 @@
       <c r="F376" t="n">
         <v>-3</v>
       </c>
-      <c r="G376" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -10714,7 +10393,6 @@
       <c r="F377" t="n">
         <v>-28</v>
       </c>
-      <c r="G377" t="inlineStr"/>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -10741,31 +10419,30 @@
       <c r="F378" t="n">
         <v>2</v>
       </c>
-      <c r="G378" t="inlineStr"/>
     </row>
     <row r="379">
-      <c r="A379" t="inlineStr">
+      <c r="A379" s="2" t="inlineStr">
         <is>
           <t>6243</t>
         </is>
       </c>
-      <c r="B379" t="inlineStr">
+      <c r="B379" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C379" t="inlineStr">
+      <c r="C379" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D379" t="n">
-        <v>0</v>
-      </c>
-      <c r="E379" t="n">
+      <c r="D379" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E379" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F379" t="n">
+      <c r="F379" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G379" t="n">
@@ -10797,7 +10474,6 @@
       <c r="F380" t="n">
         <v>-15.5</v>
       </c>
-      <c r="G380" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -10824,7 +10500,6 @@
       <c r="F381" t="n">
         <v>41</v>
       </c>
-      <c r="G381" t="inlineStr"/>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -10851,7 +10526,6 @@
       <c r="F382" t="n">
         <v>-2.5</v>
       </c>
-      <c r="G382" t="inlineStr"/>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -10878,7 +10552,6 @@
       <c r="F383" t="n">
         <v>-6</v>
       </c>
-      <c r="G383" t="inlineStr"/>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -10934,7 +10607,6 @@
       <c r="F385" t="n">
         <v>-29.5</v>
       </c>
-      <c r="G385" t="inlineStr"/>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -10961,7 +10633,6 @@
       <c r="F386" t="n">
         <v>2.5</v>
       </c>
-      <c r="G386" t="inlineStr"/>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -10988,7 +10659,6 @@
       <c r="F387" t="n">
         <v>7</v>
       </c>
-      <c r="G387" t="inlineStr"/>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -11015,7 +10685,6 @@
       <c r="F388" t="n">
         <v>-10</v>
       </c>
-      <c r="G388" t="inlineStr"/>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -11042,31 +10711,30 @@
       <c r="F389" t="n">
         <v>6</v>
       </c>
-      <c r="G389" t="inlineStr"/>
     </row>
     <row r="390">
-      <c r="A390" t="inlineStr">
+      <c r="A390" s="2" t="inlineStr">
         <is>
           <t>6243</t>
         </is>
       </c>
-      <c r="B390" t="inlineStr">
+      <c r="B390" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C390" t="inlineStr">
+      <c r="C390" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D390" t="n">
+      <c r="D390" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E390" t="n">
+      <c r="E390" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F390" t="n">
+      <c r="F390" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G390" t="n">
@@ -11098,7 +10766,6 @@
       <c r="F391" t="n">
         <v>-11</v>
       </c>
-      <c r="G391" t="inlineStr"/>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -11125,7 +10792,6 @@
       <c r="F392" t="n">
         <v>19</v>
       </c>
-      <c r="G392" t="inlineStr"/>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -11152,7 +10818,6 @@
       <c r="F393" t="n">
         <v>-9</v>
       </c>
-      <c r="G393" t="inlineStr"/>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
@@ -11179,7 +10844,6 @@
       <c r="F394" t="n">
         <v>-20</v>
       </c>
-      <c r="G394" t="inlineStr"/>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
@@ -11206,31 +10870,30 @@
       <c r="F395" t="n">
         <v>5</v>
       </c>
-      <c r="G395" t="inlineStr"/>
     </row>
     <row r="396">
-      <c r="A396" t="inlineStr">
+      <c r="A396" s="2" t="inlineStr">
         <is>
           <t>6243</t>
         </is>
       </c>
-      <c r="B396" t="inlineStr">
+      <c r="B396" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C396" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D396" t="n">
-        <v>0</v>
-      </c>
-      <c r="E396" t="n">
+      <c r="C396" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D396" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E396" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F396" t="n">
+      <c r="F396" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G396" t="n">
@@ -11262,31 +10925,30 @@
       <c r="F397" t="n">
         <v>116</v>
       </c>
-      <c r="G397" t="inlineStr"/>
     </row>
     <row r="398">
-      <c r="A398" t="inlineStr">
+      <c r="A398" s="2" t="inlineStr">
         <is>
           <t>6244</t>
         </is>
       </c>
-      <c r="B398" t="inlineStr">
+      <c r="B398" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C398" t="inlineStr">
+      <c r="C398" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D398" t="n">
-        <v>0</v>
-      </c>
-      <c r="E398" t="n">
+      <c r="D398" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E398" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="F398" t="n">
+      <c r="F398" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G398" t="n">
@@ -11318,7 +10980,6 @@
       <c r="F399" t="n">
         <v>9</v>
       </c>
-      <c r="G399" t="inlineStr"/>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -11345,7 +11006,6 @@
       <c r="F400" t="n">
         <v>8</v>
       </c>
-      <c r="G400" t="inlineStr"/>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
@@ -11372,7 +11032,6 @@
       <c r="F401" t="n">
         <v>48</v>
       </c>
-      <c r="G401" t="inlineStr"/>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -11399,7 +11058,6 @@
       <c r="F402" t="n">
         <v>4</v>
       </c>
-      <c r="G402" t="inlineStr"/>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
@@ -11426,7 +11084,6 @@
       <c r="F403" t="n">
         <v>95</v>
       </c>
-      <c r="G403" t="inlineStr"/>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
@@ -11482,7 +11139,6 @@
       <c r="F405" t="n">
         <v>4</v>
       </c>
-      <c r="G405" t="inlineStr"/>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
@@ -11509,7 +11165,6 @@
       <c r="F406" t="n">
         <v>2</v>
       </c>
-      <c r="G406" t="inlineStr"/>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
@@ -11536,7 +11191,6 @@
       <c r="F407" t="n">
         <v>8</v>
       </c>
-      <c r="G407" t="inlineStr"/>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
@@ -11592,7 +11246,6 @@
       <c r="F409" t="n">
         <v>2</v>
       </c>
-      <c r="G409" t="inlineStr"/>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
@@ -11619,31 +11272,30 @@
       <c r="F410" t="n">
         <v>144.5</v>
       </c>
-      <c r="G410" t="inlineStr"/>
     </row>
     <row r="411">
-      <c r="A411" t="inlineStr">
+      <c r="A411" s="2" t="inlineStr">
         <is>
           <t>6244</t>
         </is>
       </c>
-      <c r="B411" t="inlineStr">
+      <c r="B411" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C411" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D411" t="n">
-        <v>0</v>
-      </c>
-      <c r="E411" t="n">
+      <c r="C411" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D411" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E411" s="2" t="n">
         <v>29.5</v>
       </c>
-      <c r="F411" t="n">
+      <c r="F411" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G411" t="n">
@@ -11675,7 +11327,6 @@
       <c r="F412" t="n">
         <v>-7.5</v>
       </c>
-      <c r="G412" t="inlineStr"/>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
@@ -11702,7 +11353,6 @@
       <c r="F413" t="n">
         <v>40.5</v>
       </c>
-      <c r="G413" t="inlineStr"/>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
@@ -11729,31 +11379,30 @@
       <c r="F414" t="n">
         <v>-5</v>
       </c>
-      <c r="G414" t="inlineStr"/>
     </row>
     <row r="415">
-      <c r="A415" t="inlineStr">
+      <c r="A415" s="2" t="inlineStr">
         <is>
           <t>999999</t>
         </is>
       </c>
-      <c r="B415" t="inlineStr">
+      <c r="B415" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C415" t="inlineStr">
+      <c r="C415" s="2" t="inlineStr">
         <is>
           <t>Dec</t>
         </is>
       </c>
-      <c r="D415" t="n">
+      <c r="D415" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E415" t="n">
+      <c r="E415" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="F415" t="n">
+      <c r="F415" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G415" t="n">
@@ -11785,7 +11434,6 @@
       <c r="F416" t="n">
         <v>47</v>
       </c>
-      <c r="G416" t="inlineStr"/>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
@@ -11812,7 +11460,6 @@
       <c r="F417" t="n">
         <v>-48</v>
       </c>
-      <c r="G417" t="inlineStr"/>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
@@ -11839,31 +11486,30 @@
       <c r="F418" t="n">
         <v>5</v>
       </c>
-      <c r="G418" t="inlineStr"/>
     </row>
     <row r="419">
-      <c r="A419" t="inlineStr">
+      <c r="A419" s="2" t="inlineStr">
         <is>
           <t>999999</t>
         </is>
       </c>
-      <c r="B419" t="inlineStr">
+      <c r="B419" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C419" t="inlineStr">
+      <c r="C419" s="2" t="inlineStr">
         <is>
           <t>Feb</t>
         </is>
       </c>
-      <c r="D419" t="n">
-        <v>0</v>
-      </c>
-      <c r="E419" t="n">
+      <c r="D419" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E419" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F419" t="n">
+      <c r="F419" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G419" t="n">
@@ -11895,7 +11541,6 @@
       <c r="F420" t="n">
         <v>-5</v>
       </c>
-      <c r="G420" t="inlineStr"/>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
@@ -11922,31 +11567,30 @@
       <c r="F421" t="n">
         <v>-31</v>
       </c>
-      <c r="G421" t="inlineStr"/>
     </row>
     <row r="422">
-      <c r="A422" t="inlineStr">
+      <c r="A422" s="2" t="inlineStr">
         <is>
           <t>999999</t>
         </is>
       </c>
-      <c r="B422" t="inlineStr">
+      <c r="B422" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C422" t="inlineStr">
+      <c r="C422" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="D422" t="n">
+      <c r="D422" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E422" t="n">
+      <c r="E422" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="F422" t="n">
+      <c r="F422" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G422" t="n">
@@ -11978,7 +11622,6 @@
       <c r="F423" t="n">
         <v>-53.5</v>
       </c>
-      <c r="G423" t="inlineStr"/>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
@@ -12005,7 +11648,6 @@
       <c r="F424" t="n">
         <v>95.5</v>
       </c>
-      <c r="G424" t="inlineStr"/>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
@@ -12032,31 +11674,30 @@
       <c r="F425" t="n">
         <v>-42</v>
       </c>
-      <c r="G425" t="inlineStr"/>
     </row>
     <row r="426">
-      <c r="A426" t="inlineStr">
+      <c r="A426" s="2" t="inlineStr">
         <is>
           <t>999999</t>
         </is>
       </c>
-      <c r="B426" t="inlineStr">
+      <c r="B426" s="2" t="inlineStr">
         <is>
           <t>Vacation/leave</t>
         </is>
       </c>
-      <c r="C426" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="D426" t="n">
+      <c r="C426" s="2" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="D426" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E426" t="n">
+      <c r="E426" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F426" t="n">
+      <c r="F426" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G426" t="n">

</xml_diff>